<commit_message>
make ee measures variables
</commit_message>
<xml_diff>
--- a/projects/office_ee_Sys3.xlsx
+++ b/projects/office_ee_Sys3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="562" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="27640" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="9" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2710" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2724" uniqueCount="893">
   <si>
     <t>type</t>
   </si>
@@ -2699,6 +2699,27 @@
   </si>
   <si>
     <t>calibration_reports.gas_bill_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>[false,true]</t>
+  </si>
+  <si>
+    <t>discrete_uncertain</t>
+  </si>
+  <si>
+    <t>['EnableDCV','DisableDCV','NoChange']</t>
+  </si>
+  <si>
+    <t>['FixedDryBulb','NoEconomizer','NoChange']</t>
+  </si>
+  <si>
+    <t>NoChange</t>
+  </si>
+  <si>
+    <t>NoEconomizer</t>
+  </si>
+  <si>
+    <t>DisableDCV</t>
   </si>
 </sst>
 </file>
@@ -2876,7 +2897,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1828">
+  <cellStyleXfs count="1838">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4627,6 +4648,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4814,9 +4845,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4827,8 +4855,11 @@
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1828">
+  <cellStyles count="1838">
     <cellStyle name="Comma" xfId="1749" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -5743,6 +5774,11 @@
     <cellStyle name="Followed Hyperlink" xfId="1823" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1825" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1827" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1829" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1831" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1833" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1835" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1837" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -6656,6 +6692,11 @@
     <cellStyle name="Hyperlink" xfId="1822" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1824" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1826" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1828" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1830" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1832" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1834" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1836" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7425,9 +7466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y207"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A102:XFD126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -7440,13 +7481,14 @@
     <col min="6" max="6" width="9.6640625" style="31" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="31" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.5" style="4" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="4" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="31" customWidth="1"/>
-    <col min="11" max="11" width="8.1640625" style="31" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" style="31" customWidth="1"/>
-    <col min="13" max="14" width="7.83203125" style="31" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="31"/>
-    <col min="16" max="16" width="11.5" style="31" customWidth="1"/>
+    <col min="9" max="9" width="32.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.1640625" style="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.5" style="31" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.1640625" style="31" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="23" style="31" customWidth="1"/>
     <col min="18" max="18" width="27.6640625" style="31" customWidth="1"/>
     <col min="19" max="19" width="46.1640625" style="31" customWidth="1"/>
@@ -7481,14 +7523,14 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
-      <c r="T1" s="53" t="s">
+      <c r="T1" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="59"/>
+      <c r="X1" s="59"/>
+      <c r="Y1" s="59"/>
     </row>
     <row r="2" spans="1:25" s="8" customFormat="1" ht="15">
       <c r="A2" s="8" t="s">
@@ -9941,22 +9983,45 @@
       <c r="Q109" s="51"/>
     </row>
     <row r="110" spans="1:17">
-      <c r="B110" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D110" s="31" t="s">
+      <c r="A110" s="42"/>
+      <c r="B110" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C110" s="42"/>
+      <c r="D110" s="42" t="s">
         <v>827</v>
       </c>
-      <c r="E110" s="31" t="s">
+      <c r="E110" s="42" t="s">
         <v>826</v>
       </c>
-      <c r="F110" s="31" t="s">
+      <c r="F110" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="H110" s="31" t="b">
+      <c r="G110" s="42"/>
+      <c r="H110" s="42" t="b">
+        <v>0</v>
+      </c>
+      <c r="I110" s="42"/>
+      <c r="J110" s="45" t="b">
+        <v>0</v>
+      </c>
+      <c r="K110" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="I110" s="30"/>
+      <c r="L110" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="M110" s="44" t="b">
+        <v>0</v>
+      </c>
+      <c r="N110" s="44"/>
+      <c r="O110" s="44" t="s">
+        <v>886</v>
+      </c>
+      <c r="P110" s="42"/>
+      <c r="Q110" s="46" t="s">
+        <v>887</v>
+      </c>
     </row>
     <row r="111" spans="1:17" s="22" customFormat="1">
       <c r="A111" s="22" t="b">
@@ -10197,23 +10262,46 @@
       <c r="Q121" s="51"/>
     </row>
     <row r="122" spans="1:17">
-      <c r="B122" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D122" s="31" t="s">
+      <c r="A122" s="42"/>
+      <c r="B122" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C122" s="42"/>
+      <c r="D122" s="42" t="s">
         <v>209</v>
       </c>
-      <c r="E122" s="31" t="s">
+      <c r="E122" s="42" t="s">
         <v>823</v>
       </c>
-      <c r="F122" s="30" t="s">
+      <c r="F122" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H122" s="31" t="s">
+      <c r="G122" s="42"/>
+      <c r="H122" s="42" t="s">
         <v>822</v>
       </c>
-      <c r="I122" s="30" t="s">
+      <c r="I122" s="42" t="s">
         <v>821</v>
+      </c>
+      <c r="J122" s="42" t="s">
+        <v>892</v>
+      </c>
+      <c r="K122" s="42" t="s">
+        <v>822</v>
+      </c>
+      <c r="L122" s="42" t="s">
+        <v>890</v>
+      </c>
+      <c r="M122" s="42" t="s">
+        <v>890</v>
+      </c>
+      <c r="N122" s="42"/>
+      <c r="O122" s="42" t="s">
+        <v>888</v>
+      </c>
+      <c r="P122" s="42"/>
+      <c r="Q122" s="46" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="123" spans="1:17" s="48" customFormat="1">
@@ -10241,23 +10329,46 @@
       <c r="Q123" s="51"/>
     </row>
     <row r="124" spans="1:17">
-      <c r="B124" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="D124" s="31" t="s">
+      <c r="A124" s="42"/>
+      <c r="B124" s="42" t="s">
+        <v>22</v>
+      </c>
+      <c r="C124" s="42"/>
+      <c r="D124" s="42" t="s">
         <v>789</v>
       </c>
-      <c r="E124" s="31" t="s">
+      <c r="E124" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="F124" s="30" t="s">
+      <c r="F124" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="H124" s="31" t="s">
+      <c r="G124" s="42"/>
+      <c r="H124" s="42" t="s">
         <v>828</v>
       </c>
-      <c r="I124" s="30" t="s">
+      <c r="I124" s="42" t="s">
         <v>829</v>
+      </c>
+      <c r="J124" s="42" t="s">
+        <v>891</v>
+      </c>
+      <c r="K124" s="42" t="s">
+        <v>891</v>
+      </c>
+      <c r="L124" s="42" t="s">
+        <v>890</v>
+      </c>
+      <c r="M124" s="42" t="s">
+        <v>890</v>
+      </c>
+      <c r="N124" s="42"/>
+      <c r="O124" s="42" t="s">
+        <v>889</v>
+      </c>
+      <c r="P124" s="42"/>
+      <c r="Q124" s="46" t="s">
+        <v>887</v>
       </c>
     </row>
     <row r="125" spans="1:17">
@@ -10645,9 +10756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:L33"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -10664,920 +10775,920 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18">
-      <c r="A1" s="55"/>
-      <c r="B1" s="55"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="56" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="55" t="s">
         <v>467</v>
       </c>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="54"/>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:12" s="8" customFormat="1" ht="15">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="56" t="s">
         <v>459</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="57" t="s">
         <v>637</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="56" t="s">
         <v>460</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E2" s="56" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F2" s="56" t="s">
         <v>622</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G2" s="56" t="s">
         <v>623</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H2" s="56" t="s">
         <v>624</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I2" s="56" t="s">
         <v>625</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>626</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K2" s="56" t="s">
         <v>627</v>
       </c>
-      <c r="L2" s="57"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="57" t="s">
         <v>628</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="57" t="s">
         <v>642</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="57" t="s">
         <v>631</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58" t="s">
+      <c r="D3" s="57"/>
+      <c r="E3" s="57" t="s">
         <v>629</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="F3" s="57" t="s">
         <v>461</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="57" t="s">
         <v>461</v>
       </c>
-      <c r="H3" s="58" t="s">
+      <c r="H3" s="57" t="s">
         <v>461</v>
       </c>
-      <c r="I3" s="58" t="s">
+      <c r="I3" s="57" t="s">
         <v>619</v>
       </c>
-      <c r="J3" s="59" t="s">
+      <c r="J3" s="58" t="s">
         <v>619</v>
       </c>
-      <c r="K3" s="58" t="s">
+      <c r="K3" s="57" t="s">
         <v>630</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="57" t="s">
         <v>643</v>
       </c>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="53" t="s">
         <v>644</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="53" t="s">
         <v>638</v>
       </c>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="53" t="s">
         <v>634</v>
       </c>
-      <c r="D4" s="54" t="s">
+      <c r="D4" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F4" s="54" t="b">
+      <c r="F4" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="54" t="b">
+      <c r="G4" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H4" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="54"/>
-      <c r="J4" s="54"/>
-      <c r="K4" s="54"/>
-      <c r="L4" s="54"/>
+      <c r="H4" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="A5" s="54" t="s">
+      <c r="A5" s="53" t="s">
         <v>645</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="53" t="s">
         <v>639</v>
       </c>
-      <c r="C5" s="54" t="s">
+      <c r="C5" s="53" t="s">
         <v>635</v>
       </c>
-      <c r="D5" s="54" t="s">
+      <c r="D5" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F5" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" s="54" t="b">
+      <c r="F5" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H5" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="54"/>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
+      <c r="H5" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="53" t="s">
         <v>646</v>
       </c>
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="53" t="s">
         <v>641</v>
       </c>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="53" t="s">
         <v>632</v>
       </c>
-      <c r="D6" s="54" t="s">
+      <c r="D6" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F6" s="54" t="b">
+      <c r="F6" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="54" t="b">
+      <c r="G6" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H6" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
+      <c r="H6" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="53" t="s">
         <v>647</v>
       </c>
-      <c r="B7" s="54" t="s">
+      <c r="B7" s="53" t="s">
         <v>640</v>
       </c>
-      <c r="C7" s="54" t="s">
+      <c r="C7" s="53" t="s">
         <v>633</v>
       </c>
-      <c r="D7" s="54" t="s">
+      <c r="D7" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E7" s="54" t="s">
+      <c r="E7" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F7" s="54" t="b">
+      <c r="F7" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="54" t="b">
+      <c r="G7" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H7" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I7" s="54"/>
-      <c r="J7" s="54"/>
-      <c r="K7" s="54"/>
-      <c r="L7" s="54"/>
+      <c r="H7" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="54" t="s">
+      <c r="A8" s="53" t="s">
         <v>838</v>
       </c>
-      <c r="B8" s="54"/>
-      <c r="C8" s="54" t="s">
+      <c r="B8" s="53"/>
+      <c r="C8" s="53" t="s">
         <v>839</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G8" s="54" t="b">
+      <c r="F8" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H8" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="54"/>
-      <c r="L8" s="54"/>
+      <c r="H8" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
     </row>
     <row r="9" spans="1:12">
-      <c r="A9" s="54" t="s">
+      <c r="A9" s="53" t="s">
         <v>840</v>
       </c>
-      <c r="B9" s="54"/>
-      <c r="C9" s="54" t="s">
+      <c r="B9" s="53"/>
+      <c r="C9" s="53" t="s">
         <v>841</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E9" s="54" t="s">
+      <c r="E9" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="54" t="b">
+      <c r="F9" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H9" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="54"/>
-      <c r="J9" s="54"/>
-      <c r="K9" s="54"/>
-      <c r="L9" s="54"/>
+      <c r="H9" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="53"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="53"/>
+      <c r="L9" s="53"/>
     </row>
     <row r="10" spans="1:12">
-      <c r="A10" s="54" t="s">
+      <c r="A10" s="53" t="s">
         <v>842</v>
       </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54" t="s">
+      <c r="B10" s="53"/>
+      <c r="C10" s="53" t="s">
         <v>843</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E10" s="54" t="s">
+      <c r="E10" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F10" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G10" s="54" t="b">
+      <c r="F10" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H10" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="54"/>
-      <c r="K10" s="54"/>
-      <c r="L10" s="54"/>
+      <c r="H10" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
     </row>
     <row r="11" spans="1:12">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="53" t="s">
         <v>844</v>
       </c>
-      <c r="B11" s="54"/>
-      <c r="C11" s="54" t="s">
+      <c r="B11" s="53"/>
+      <c r="C11" s="53" t="s">
         <v>845</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E11" s="54" t="s">
+      <c r="E11" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" s="54" t="b">
+      <c r="F11" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H11" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
+      <c r="H11" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
     </row>
     <row r="12" spans="1:12">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="53" t="s">
         <v>846</v>
       </c>
-      <c r="B12" s="54"/>
-      <c r="C12" s="54" t="s">
+      <c r="B12" s="53"/>
+      <c r="C12" s="53" t="s">
         <v>847</v>
       </c>
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E12" s="54" t="s">
+      <c r="E12" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F12" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" s="54" t="b">
+      <c r="F12" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H12" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I12" s="54"/>
-      <c r="J12" s="54"/>
-      <c r="K12" s="54"/>
-      <c r="L12" s="54"/>
+      <c r="H12" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I12" s="53"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
     </row>
     <row r="13" spans="1:12">
-      <c r="A13" s="54" t="s">
+      <c r="A13" s="53" t="s">
         <v>848</v>
       </c>
-      <c r="B13" s="54"/>
-      <c r="C13" s="54" t="s">
+      <c r="B13" s="53"/>
+      <c r="C13" s="53" t="s">
         <v>849</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E13" s="54" t="s">
+      <c r="E13" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" s="54" t="b">
+      <c r="F13" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
-      <c r="L13" s="54"/>
+      <c r="H13" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I13" s="53"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
     </row>
     <row r="14" spans="1:12">
-      <c r="A14" s="54" t="s">
+      <c r="A14" s="53" t="s">
         <v>850</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54" t="s">
+      <c r="B14" s="53"/>
+      <c r="C14" s="53" t="s">
         <v>851</v>
       </c>
-      <c r="D14" s="54" t="s">
+      <c r="D14" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E14" s="54" t="s">
+      <c r="E14" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="54" t="b">
+      <c r="F14" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H14" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="54"/>
-      <c r="L14" s="54"/>
+      <c r="H14" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
     </row>
     <row r="15" spans="1:12">
-      <c r="A15" s="54" t="s">
+      <c r="A15" s="53" t="s">
         <v>852</v>
       </c>
-      <c r="B15" s="54"/>
-      <c r="C15" s="54" t="s">
+      <c r="B15" s="53"/>
+      <c r="C15" s="53" t="s">
         <v>853</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" s="54" t="b">
+      <c r="F15" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H15" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="54"/>
-      <c r="L15" s="54"/>
+      <c r="H15" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
     </row>
     <row r="16" spans="1:12">
-      <c r="A16" s="54" t="s">
+      <c r="A16" s="53" t="s">
         <v>854</v>
       </c>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54" t="s">
+      <c r="B16" s="53"/>
+      <c r="C16" s="53" t="s">
         <v>855</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="D16" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E16" s="54" t="s">
+      <c r="E16" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="54" t="b">
+      <c r="F16" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H16" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
-      <c r="K16" s="54"/>
-      <c r="L16" s="54"/>
+      <c r="H16" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
     </row>
     <row r="17" spans="1:12">
-      <c r="A17" s="54" t="s">
+      <c r="A17" s="53" t="s">
         <v>856</v>
       </c>
-      <c r="B17" s="54"/>
-      <c r="C17" s="54" t="s">
+      <c r="B17" s="53"/>
+      <c r="C17" s="53" t="s">
         <v>857</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E17" s="54" t="s">
+      <c r="E17" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" s="54" t="b">
+      <c r="F17" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H17" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="54"/>
-      <c r="L17" s="54"/>
+      <c r="H17" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="54" t="s">
+      <c r="A18" s="53" t="s">
         <v>858</v>
       </c>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54" t="s">
+      <c r="B18" s="53"/>
+      <c r="C18" s="53" t="s">
         <v>859</v>
       </c>
-      <c r="D18" s="54" t="s">
+      <c r="D18" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E18" s="54" t="s">
+      <c r="E18" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" s="54" t="b">
+      <c r="F18" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H18" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="54"/>
-      <c r="L18" s="54"/>
+      <c r="H18" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="53"/>
+      <c r="L18" s="53"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="54" t="s">
+      <c r="A19" s="53" t="s">
         <v>860</v>
       </c>
-      <c r="B19" s="54"/>
-      <c r="C19" s="54" t="s">
+      <c r="B19" s="53"/>
+      <c r="C19" s="53" t="s">
         <v>861</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E19" s="54" t="s">
+      <c r="E19" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" s="54" t="b">
+      <c r="F19" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I19" s="54"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="54"/>
-      <c r="L19" s="54"/>
+      <c r="H19" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="54" t="s">
+      <c r="A20" s="53" t="s">
         <v>862</v>
       </c>
-      <c r="B20" s="54"/>
-      <c r="C20" s="54" t="s">
+      <c r="B20" s="53"/>
+      <c r="C20" s="53" t="s">
         <v>863</v>
       </c>
-      <c r="D20" s="54" t="s">
+      <c r="D20" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E20" s="54" t="s">
+      <c r="E20" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="54" t="b">
+      <c r="F20" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H20" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="54"/>
-      <c r="J20" s="54"/>
-      <c r="K20" s="54"/>
-      <c r="L20" s="54"/>
+      <c r="H20" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="53"/>
+      <c r="J20" s="53"/>
+      <c r="K20" s="53"/>
+      <c r="L20" s="53"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="54" t="s">
+      <c r="A21" s="53" t="s">
         <v>864</v>
       </c>
-      <c r="B21" s="54"/>
-      <c r="C21" s="54" t="s">
+      <c r="B21" s="53"/>
+      <c r="C21" s="53" t="s">
         <v>865</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="53" t="s">
         <v>468</v>
       </c>
-      <c r="E21" s="54" t="s">
+      <c r="E21" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G21" s="54" t="b">
+      <c r="F21" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H21" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I21" s="54"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="54"/>
-      <c r="L21" s="54"/>
+      <c r="H21" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I21" s="53"/>
+      <c r="J21" s="53"/>
+      <c r="K21" s="53"/>
+      <c r="L21" s="53"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="54" t="s">
+      <c r="A22" s="53" t="s">
         <v>866</v>
       </c>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54" t="s">
+      <c r="B22" s="53"/>
+      <c r="C22" s="53" t="s">
         <v>867</v>
       </c>
-      <c r="D22" s="54" t="s">
+      <c r="D22" s="53" t="s">
         <v>868</v>
       </c>
-      <c r="E22" s="54" t="s">
+      <c r="E22" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F22" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G22" s="54" t="b">
+      <c r="F22" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H22" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="54"/>
-      <c r="L22" s="54"/>
+      <c r="H22" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="54" t="s">
+      <c r="A23" s="53" t="s">
         <v>869</v>
       </c>
-      <c r="B23" s="54"/>
-      <c r="C23" s="54" t="s">
+      <c r="B23" s="53"/>
+      <c r="C23" s="53" t="s">
         <v>870</v>
       </c>
-      <c r="D23" s="54" t="s">
+      <c r="D23" s="53" t="s">
         <v>868</v>
       </c>
-      <c r="E23" s="54" t="s">
+      <c r="E23" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F23" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" s="54" t="b">
+      <c r="F23" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H23" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="54"/>
-      <c r="J23" s="54"/>
-      <c r="K23" s="54"/>
-      <c r="L23" s="54"/>
+      <c r="H23" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I23" s="53"/>
+      <c r="J23" s="53"/>
+      <c r="K23" s="53"/>
+      <c r="L23" s="53"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="54" t="s">
+      <c r="A24" s="53" t="s">
         <v>871</v>
       </c>
-      <c r="B24" s="54"/>
-      <c r="C24" s="54" t="s">
+      <c r="B24" s="53"/>
+      <c r="C24" s="53" t="s">
         <v>872</v>
       </c>
-      <c r="D24" s="54" t="s">
+      <c r="D24" s="53" t="s">
         <v>868</v>
       </c>
-      <c r="E24" s="54" t="s">
+      <c r="E24" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F24" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="G24" s="54" t="b">
+      <c r="F24" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="G24" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H24" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I24" s="54"/>
-      <c r="J24" s="54"/>
-      <c r="K24" s="54"/>
-      <c r="L24" s="54"/>
+      <c r="H24" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I24" s="53"/>
+      <c r="J24" s="53"/>
+      <c r="K24" s="53"/>
+      <c r="L24" s="53"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="54" t="s">
+      <c r="A25" s="53" t="s">
         <v>873</v>
       </c>
-      <c r="B25" s="54"/>
-      <c r="C25" s="54" t="s">
+      <c r="B25" s="53"/>
+      <c r="C25" s="53" t="s">
         <v>874</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="53" t="s">
         <v>875</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F25" s="54" t="b">
+      <c r="F25" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G25" s="54" t="b">
+      <c r="G25" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H25" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="54"/>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
+      <c r="H25" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="53"/>
+      <c r="J25" s="53"/>
+      <c r="K25" s="53"/>
+      <c r="L25" s="53"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="54" t="s">
+      <c r="A26" s="53" t="s">
         <v>706</v>
       </c>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54" t="s">
+      <c r="B26" s="53"/>
+      <c r="C26" s="53" t="s">
         <v>876</v>
       </c>
-      <c r="D26" s="54" t="s">
+      <c r="D26" s="53" t="s">
         <v>707</v>
       </c>
-      <c r="E26" s="54" t="s">
+      <c r="E26" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F26" s="54" t="b">
+      <c r="F26" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G26" s="54" t="b">
+      <c r="G26" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H26" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="54"/>
-      <c r="L26" s="54"/>
+      <c r="H26" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="53"/>
+      <c r="L26" s="53"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="54" t="s">
+      <c r="A27" s="53" t="s">
         <v>708</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54" t="s">
+      <c r="B27" s="53"/>
+      <c r="C27" s="53" t="s">
         <v>877</v>
       </c>
-      <c r="D27" s="54" t="s">
+      <c r="D27" s="53" t="s">
         <v>709</v>
       </c>
-      <c r="E27" s="54" t="s">
+      <c r="E27" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="54" t="b">
+      <c r="F27" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G27" s="54" t="b">
+      <c r="G27" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H27" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="54"/>
-      <c r="J27" s="54"/>
-      <c r="K27" s="54"/>
-      <c r="L27" s="54"/>
+      <c r="H27" s="53" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="53"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="53"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="53" t="s">
         <v>878</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54" t="s">
+      <c r="B28" s="53"/>
+      <c r="C28" s="53" t="s">
         <v>879</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="53" t="s">
         <v>769</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F28" s="54" t="b">
+      <c r="F28" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G28" s="54" t="b">
+      <c r="G28" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H28" s="54" t="b">
+      <c r="H28" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="I28" s="54">
-        <v>0</v>
-      </c>
-      <c r="J28" s="54"/>
-      <c r="K28" s="54"/>
-      <c r="L28" s="54"/>
+      <c r="I28" s="53">
+        <v>0</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="53" t="s">
         <v>880</v>
       </c>
-      <c r="B29" s="54"/>
-      <c r="C29" s="54" t="s">
+      <c r="B29" s="53"/>
+      <c r="C29" s="53" t="s">
         <v>881</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D29" s="53" t="s">
         <v>769</v>
       </c>
-      <c r="E29" s="54" t="s">
+      <c r="E29" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F29" s="54" t="b">
+      <c r="F29" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G29" s="54" t="b">
+      <c r="G29" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H29" s="54" t="b">
+      <c r="H29" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="I29" s="54">
-        <v>0</v>
-      </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
+      <c r="I29" s="53">
+        <v>0</v>
+      </c>
+      <c r="J29" s="53"/>
+      <c r="K29" s="53"/>
+      <c r="L29" s="53"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="54" t="s">
+      <c r="A30" s="53" t="s">
         <v>882</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54" t="s">
+      <c r="B30" s="53"/>
+      <c r="C30" s="53" t="s">
         <v>883</v>
       </c>
-      <c r="D30" s="54" t="s">
+      <c r="D30" s="53" t="s">
         <v>769</v>
       </c>
-      <c r="E30" s="54" t="s">
+      <c r="E30" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F30" s="54" t="b">
+      <c r="F30" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G30" s="54" t="b">
+      <c r="G30" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H30" s="54" t="b">
+      <c r="H30" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="I30" s="54">
-        <v>0</v>
-      </c>
-      <c r="J30" s="54"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="I30" s="53">
+        <v>0</v>
+      </c>
+      <c r="J30" s="53"/>
+      <c r="K30" s="53"/>
+      <c r="L30" s="53"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="54" t="s">
+      <c r="A31" s="53" t="s">
         <v>884</v>
       </c>
-      <c r="B31" s="54"/>
-      <c r="C31" s="54" t="s">
+      <c r="B31" s="53"/>
+      <c r="C31" s="53" t="s">
         <v>885</v>
       </c>
-      <c r="D31" s="54" t="s">
+      <c r="D31" s="53" t="s">
         <v>769</v>
       </c>
-      <c r="E31" s="54" t="s">
+      <c r="E31" s="53" t="s">
         <v>64</v>
       </c>
-      <c r="F31" s="54" t="b">
+      <c r="F31" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="G31" s="54" t="b">
+      <c r="G31" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="H31" s="54" t="b">
+      <c r="H31" s="53" t="b">
         <v>1</v>
       </c>
-      <c r="I31" s="54">
-        <v>0</v>
-      </c>
-      <c r="J31" s="54"/>
-      <c r="K31" s="54"/>
-      <c r="L31" s="54"/>
+      <c r="I31" s="53">
+        <v>0</v>
+      </c>
+      <c r="J31" s="53"/>
+      <c r="K31" s="53"/>
+      <c r="L31" s="53"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="54"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="54"/>
-      <c r="D32" s="54"/>
-      <c r="E32" s="54"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="54"/>
-      <c r="L32" s="54"/>
+      <c r="A32" s="53"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="53"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="L32" s="53"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="54"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="54"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="54"/>
-      <c r="I33" s="54"/>
-      <c r="J33" s="54"/>
-      <c r="K33" s="54"/>
-      <c r="L33" s="54"/>
+      <c r="A33" s="53"/>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="53"/>
+      <c r="L33" s="53"/>
     </row>
     <row r="34" spans="1:12">
       <c r="A34" s="30"/>

</xml_diff>